<commit_message>
ScreenShots for all Execution Classes
</commit_message>
<xml_diff>
--- a/BookStore/External Files/Book1.xlsx
+++ b/BookStore/External Files/Book1.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="21015" windowHeight="11250"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11910" windowHeight="6090" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:J10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>SI No</t>
   </si>
@@ -46,6 +46,12 @@
     <t>gopikuncham</t>
   </si>
   <si>
+    <t>gksaka</t>
+  </si>
+  <si>
+    <t>fg</t>
+  </si>
+  <si>
     <t>gk030994@gmail.com</t>
   </si>
   <si>
@@ -101,27 +107,6 @@
   </si>
   <si>
     <t>Andhra Pradesh</t>
-  </si>
-  <si>
-    <t>gjajgs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type </t>
-  </si>
-  <si>
-    <t>Negative</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>vmsa</t>
-  </si>
-  <si>
-    <t>pass</t>
   </si>
 </sst>
 </file>
@@ -150,7 +135,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,12 +145,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -186,12 +165,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -487,24 +465,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -521,13 +499,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="4" t="s">
-        <v>30</v>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -538,19 +513,16 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>28</v>
+      <c r="E2">
+        <v>9553617</v>
       </c>
       <c r="F2">
         <v>121</v>
       </c>
-      <c r="G2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
-        <v>30</v>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -559,48 +531,21 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3">
-        <v>4575</v>
-      </c>
-      <c r="G3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <v>9553191317</v>
-      </c>
-      <c r="F4">
-        <v>54210</v>
-      </c>
-      <c r="G4" t="s">
-        <v>34</v>
+      <c r="F3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -608,14 +553,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -623,10 +568,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -637,7 +582,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -666,15 +611,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -682,31 +627,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K1" s="1"/>
     </row>
@@ -715,47 +660,35 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H2">
         <v>500072</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>